<commit_message>
filtering drives based on the cutOff
</commit_message>
<xml_diff>
--- a/public/temp/userData_lates.xlsx
+++ b/public/temp/userData_lates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c2ce842ce4e0359/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91934\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{15B3B264-98CC-4C02-A937-5F0920EA46DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A91D70C3-328D-45FA-86C6-C4EA0045818D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C414F1C7-4E78-4069-BE1D-7D28F1411844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{06FDC64D-9342-4DE7-B0AB-52CF345A1314}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>userName</t>
   </si>
@@ -42,37 +42,22 @@
     <t>password</t>
   </si>
   <si>
-    <t>sirisha</t>
-  </si>
-  <si>
-    <t>s.sirisha</t>
-  </si>
-  <si>
-    <t>20l31a02f9</t>
-  </si>
-  <si>
     <t>personalEmail</t>
   </si>
   <si>
-    <t>20l31a02f9@vignaniit.edu.in</t>
-  </si>
-  <si>
     <t>s.sruthi</t>
   </si>
   <si>
-    <t>20l31a02f7</t>
-  </si>
-  <si>
-    <t>sirisha@gmail.com</t>
-  </si>
-  <si>
     <t>srithi@gmail.com</t>
   </si>
   <si>
-    <t>20l31a02f7@vignaniit.edu.in</t>
-  </si>
-  <si>
     <t>sruthi</t>
+  </si>
+  <si>
+    <t>20l31a02f8@vignaniit.edu.in</t>
+  </si>
+  <si>
+    <t>20l31a02f8</t>
   </si>
 </sst>
 </file>
@@ -467,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96693750-3E03-432B-8423-3FF7B24DEFA2}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,48 +478,33 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -542,9 +512,6 @@
     <hyperlink ref="B2" r:id="rId1" display="aha@gmail.com" xr:uid="{05926F65-EB5E-48CE-A86F-EABC3B7D9257}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{8A3CF0A5-886D-4BB1-AD34-7DE23C0BDB86}"/>
     <hyperlink ref="F2" r:id="rId3" xr:uid="{205B763E-5358-4476-B400-D66796C18846}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{108E6ED6-8F1B-450A-890D-B414123BBBC2}"/>
-    <hyperlink ref="F3" r:id="rId5" xr:uid="{8AE6A40C-87A3-4490-AD4A-FA258B3FEE03}"/>
-    <hyperlink ref="B3" r:id="rId6" display="aha@gmail.com" xr:uid="{60EDC99D-5D25-47B9-B547-E682A245A279}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>